<commit_message>
Add new columns in the requests report.
</commit_message>
<xml_diff>
--- a/reports/requests_report/templates/xlsx/template.xlsx
+++ b/reports/requests_report/templates/xlsx/template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\vendor_subscriptions_report\reports\requests_report\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\global-connect-reports\reports\requests_report\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DAFE8F-E37A-40C3-99EB-3B6A4108FBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD40101-C29B-405E-BF74-BBBEAC2DBEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17856" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$G$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$G$1:$X$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Exported At</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Item ID</t>
+  </si>
+  <si>
+    <t>Vendor ID</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>HUB Name</t>
+  </si>
+  <si>
+    <t>HUB ID</t>
   </si>
 </sst>
 </file>
@@ -435,10 +447,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -446,16 +458,16 @@
     <col min="2" max="3" width="25.77734375" customWidth="1" outlineLevel="1"/>
     <col min="4" max="10" width="21.6640625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="45.77734375" customWidth="1"/>
-    <col min="13" max="14" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="45.77734375" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" customWidth="1"/>
-    <col min="18" max="19" width="21.21875" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="21.21875" customWidth="1"/>
+    <col min="12" max="14" width="45.77734375" customWidth="1"/>
+    <col min="15" max="16" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="19" width="45.77734375" customWidth="1"/>
+    <col min="20" max="20" width="18.109375" customWidth="1"/>
+    <col min="21" max="21" width="18.44140625" customWidth="1"/>
+    <col min="22" max="23" width="21.21875" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -489,32 +501,44 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:T1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="G1:X1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>